<commit_message>
edited sprint 2 backlogs and product backlog too.
</commit_message>
<xml_diff>
--- a/elsa/sprint2/doc/Scrum_ELSA_Sprint_2.xlsx
+++ b/elsa/sprint2/doc/Scrum_ELSA_Sprint_2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="159">
   <si>
     <t xml:space="preserve">Product Name:</t>
   </si>
@@ -83,6 +83,9 @@
     <t xml:space="preserve">...and so on</t>
   </si>
   <si>
+    <t xml:space="preserve">I was going to edit it but don’t know what is coming in sprint 3 so, didn’t edit it at all.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Note: Priority and specs for unfinished Features is subject to change at the end of each sprint at the whim of the Product Owner</t>
   </si>
   <si>
@@ -161,6 +164,9 @@
     <t xml:space="preserve">ORDER</t>
   </si>
   <si>
+    <t xml:space="preserve">Finished in Sprint 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Associate a customer with one or more desktops into an order</t>
   </si>
   <si>
@@ -218,6 +224,9 @@
     <t xml:space="preserve">SAVE</t>
   </si>
   <si>
+    <t xml:space="preserve">In Test</t>
+  </si>
+  <si>
     <t xml:space="preserve">Manager</t>
   </si>
   <si>
@@ -456,6 +465,39 @@
   </si>
   <si>
     <t xml:space="preserve">Ensure ALL CODE is on GitHub by deadline!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint 2 took me about 3 days in total.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I wrote my .h files in a day.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Took a breaj for a few days and then resumed in weekend again.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">And, finally finished everything on Monday night.</t>
   </si>
   <si>
     <t xml:space="preserve">--&gt; Add tasks to complete each feature for this sprint</t>
@@ -470,7 +512,7 @@
     <numFmt numFmtId="165" formatCode="MMM\ DD"/>
     <numFmt numFmtId="166" formatCode="MM/DD/YY\ HH:MM\ AM/PM"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -493,8 +535,9 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
+      <b val="true"/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -502,88 +545,6 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -607,6 +568,14 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -650,12 +619,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF98FB98"/>
+        <bgColor rgb="FF99FF66"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -665,74 +640,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF666699"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FFFF0000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF98FB98"/>
-        <bgColor rgb="FF99FF66"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC0C0C0"/>
         <bgColor rgb="FFB3B3B3"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -765,7 +683,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -789,57 +707,6 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="8" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="47">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -850,7 +717,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -858,23 +725,23 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -882,7 +749,7 @@
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -894,19 +761,19 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -914,55 +781,55 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -974,7 +841,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -982,7 +849,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1002,23 +869,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1026,35 +893,18 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Accent 1 17" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 16" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2 18" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3 19" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad 13" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error 15" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote 8" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good 11" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1 4" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2 5" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 3" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Hyperlink 9" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral 12" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note 7" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status 10" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text 6" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning 14" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1062,14 +912,14 @@
       <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000EE"/>
+      <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FFCC0000"/>
-      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
@@ -1077,11 +927,11 @@
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FF98FB98"/>
+      <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -1092,12 +942,12 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FF98FB98"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99FF66"/>
@@ -1119,7 +969,1100 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Product Backlog Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0822345810160595"/>
+          <c:y val="0.161975370696155"/>
+          <c:w val="0.88420921077298"/>
+          <c:h val="0.635586830862026"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="line"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Product Backlog'!$A$12:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Product Backlog'!$B$12:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="14448316"/>
+        <c:axId val="35832246"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="14448316"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="6"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Sprints</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="35832246"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="35832246"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Features Remaining at end of Sprint</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="14448316"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Sprint Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 01 Backlog'!$B$7:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="64188524"/>
+        <c:axId val="66746464"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="64188524"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Days</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="66746464"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="66746464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="64188524"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Sprint Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 02 Backlog'!$B$7:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="45861015"/>
+        <c:axId val="17021155"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="45861015"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Days</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="17021155"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="17021155"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="45861015"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Sprint Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 03 Backlog'!$B$7:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="67761763"/>
+        <c:axId val="84525947"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="67761763"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Days</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="84525947"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="84525947"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="67761763"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1227,11 +2170,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="26217827"/>
-        <c:axId val="31970491"/>
+        <c:axId val="2751188"/>
+        <c:axId val="2289460"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="26217827"/>
+        <c:axId val="2751188"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1287,14 +2230,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31970491"/>
+        <c:crossAx val="2289460"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="31970491"/>
+        <c:axId val="2289460"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1359,1100 +2302,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26217827"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Product Backlog Burn Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.0822294426393402"/>
-          <c:y val="0.161955019474808"/>
-          <c:w val="0.884278930267433"/>
-          <c:h val="0.63563261716296"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:scatterChart>
-        <c:scatterStyle val="line"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:numFmt formatCode="General" sourceLinked="1"/>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Product Backlog'!$A$12:$A$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Product Backlog'!$B$12:$B$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>18</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:axId val="18117207"/>
-        <c:axId val="30782174"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="18117207"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="6"/>
-          <c:min val="0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Sprints</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="30782174"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="30782174"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Features Remaining at end of Sprint</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="18117207"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="span"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Sprint Burn Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:numFmt formatCode="General" sourceLinked="1"/>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sprint 01 Backlog'!$B$7:$B$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>16</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="29275560"/>
-        <c:axId val="17515211"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="29275560"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Days</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="17515211"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="17515211"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Tasks</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="29275560"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Sprint Burn Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:numFmt formatCode="General" sourceLinked="1"/>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sprint 02 Backlog'!$B$7:$B$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="50694645"/>
-        <c:axId val="65132304"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="50694645"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Days</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="65132304"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="65132304"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Tasks</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="50694645"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Sprint Burn Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:numFmt formatCode="General" sourceLinked="1"/>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sprint 03 Backlog'!$B$7:$B$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="95133697"/>
-        <c:axId val="21994383"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="95133697"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Days</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="21994383"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="21994383"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Tasks</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="95133697"/>
+        <c:crossAx val="2751188"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2490,9 +2340,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>4187880</xdr:colOff>
+      <xdr:colOff>4187520</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>133920</xdr:rowOff>
+      <xdr:rowOff>133560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2501,7 +2351,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="11400480" y="443160"/>
-        <a:ext cx="5761080" cy="2864880"/>
+        <a:ext cx="5760720" cy="2864520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2525,9 +2375,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1772640</xdr:colOff>
+      <xdr:colOff>1772280</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>132120</xdr:rowOff>
+      <xdr:rowOff>131760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2536,7 +2386,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="4086360" y="448560"/>
-        <a:ext cx="3751560" cy="1854360"/>
+        <a:ext cx="3751920" cy="1854000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2556,7 +2406,7 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>1679760</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>65880</xdr:rowOff>
+      <xdr:rowOff>66240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
@@ -2570,8 +2420,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4086360" y="448560"/>
-        <a:ext cx="3751920" cy="1854360"/>
+        <a:off x="4086360" y="448920"/>
+        <a:ext cx="3752280" cy="1854000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2595,9 +2445,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518040</xdr:colOff>
+      <xdr:colOff>517680</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>132120</xdr:rowOff>
+      <xdr:rowOff>131760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2606,7 +2456,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="4086360" y="448560"/>
-        <a:ext cx="3751920" cy="1854360"/>
+        <a:ext cx="3751920" cy="1854000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2630,9 +2480,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518040</xdr:colOff>
+      <xdr:colOff>517680</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>132120</xdr:rowOff>
+      <xdr:rowOff>131760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2641,7 +2491,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="4086360" y="448560"/>
-        <a:ext cx="3751920" cy="1854360"/>
+        <a:ext cx="3751920" cy="1854000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2663,7 +2513,7 @@
   <dimension ref="A1:K95"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
+      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2873,11 +2723,11 @@
       </c>
       <c r="B13" s="3" t="n">
         <f aca="false">B12-C13</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C13" s="10" t="n">
         <f aca="false">COUNTIF(G$24:G$101,"Finished in Sprint 1")</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="11"/>
@@ -2901,7 +2751,7 @@
       </c>
       <c r="C14" s="10" t="n">
         <f aca="false">COUNTIF(G$24:G$101,"Finished in Sprint 2")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="11"/>
@@ -2974,7 +2824,9 @@
       <c r="D17" s="10"/>
       <c r="E17" s="11"/>
       <c r="F17" s="13"/>
-      <c r="G17" s="3"/>
+      <c r="G17" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
@@ -3012,7 +2864,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
@@ -3026,7 +2878,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
@@ -3038,7 +2890,7 @@
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
       <c r="F22" s="16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G22" s="16"/>
       <c r="H22" s="15"/>
@@ -3047,42 +2899,42 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C23" s="18" t="s">
         <v>7</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F23" s="18" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H23" s="18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I23" s="18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J23" s="18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K23" s="18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="19" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B24" s="20" t="n">
         <v>1</v>
@@ -3098,22 +2950,22 @@
         <v>1</v>
       </c>
       <c r="G24" s="22" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H24" s="23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I24" s="24" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J24" s="24" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K24" s="24"/>
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="19" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B25" s="20" t="n">
         <v>2</v>
@@ -3129,22 +2981,22 @@
         <v>4</v>
       </c>
       <c r="G25" s="22" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H25" s="23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I25" s="24" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J25" s="24" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K25" s="24"/>
     </row>
     <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="19" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B26" s="20" t="n">
         <v>3</v>
@@ -3160,22 +3012,22 @@
         <v>1</v>
       </c>
       <c r="G26" s="22" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H26" s="23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I26" s="24" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J26" s="24" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K26" s="24"/>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="19" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B27" s="20" t="n">
         <v>4</v>
@@ -3191,22 +3043,22 @@
         <v>3</v>
       </c>
       <c r="G27" s="22" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="H27" s="23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I27" s="24" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J27" s="24" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K27" s="24"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="25" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B28" s="26" t="n">
         <v>5</v>
@@ -3221,21 +3073,21 @@
       <c r="F28" s="21"/>
       <c r="G28" s="22"/>
       <c r="H28" s="23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I28" s="24" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="J28" s="24" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="K28" s="24" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="25" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B29" s="26" t="n">
         <v>6</v>
@@ -3250,21 +3102,21 @@
       <c r="F29" s="21"/>
       <c r="G29" s="22"/>
       <c r="H29" s="23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I29" s="24" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="J29" s="24" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="K29" s="24" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="25" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B30" s="26" t="n">
         <v>7</v>
@@ -3279,21 +3131,21 @@
       <c r="F30" s="21"/>
       <c r="G30" s="22"/>
       <c r="H30" s="23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="J30" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K30" s="24" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="25" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B31" s="26" t="n">
         <v>8</v>
@@ -3308,19 +3160,19 @@
       <c r="F31" s="21"/>
       <c r="G31" s="22"/>
       <c r="H31" s="23" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I31" s="24" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="J31" s="24" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K31" s="24"/>
     </row>
     <row r="32" s="27" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="19" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B32" s="20" t="n">
         <v>9</v>
@@ -3333,23 +3185,25 @@
         <v>13</v>
       </c>
       <c r="F32" s="21"/>
-      <c r="G32" s="22"/>
+      <c r="G32" s="22" t="s">
+        <v>66</v>
+      </c>
       <c r="H32" s="23" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I32" s="24" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="J32" s="24" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="K32" s="24" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="19" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B33" s="20" t="n">
         <v>10</v>
@@ -3364,21 +3218,21 @@
       <c r="F33" s="21"/>
       <c r="G33" s="22"/>
       <c r="H33" s="23" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I33" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="J33" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="J33" s="24" t="s">
-        <v>66</v>
-      </c>
       <c r="K33" s="24" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="19" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B34" s="20" t="n">
         <v>11</v>
@@ -3393,21 +3247,21 @@
       <c r="F34" s="21"/>
       <c r="G34" s="22"/>
       <c r="H34" s="23" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I34" s="24" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="J34" s="24" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="K34" s="24" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="25" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B35" s="26" t="n">
         <v>12</v>
@@ -3422,19 +3276,19 @@
       <c r="F35" s="21"/>
       <c r="G35" s="22"/>
       <c r="H35" s="23" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="I35" s="24" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J35" s="24" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K35" s="24"/>
     </row>
     <row r="36" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="25" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B36" s="26" t="n">
         <v>13</v>
@@ -3449,13 +3303,13 @@
       <c r="F36" s="21"/>
       <c r="G36" s="22"/>
       <c r="H36" s="23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I36" s="24" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="J36" s="24" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="K36" s="24"/>
     </row>
@@ -3482,7 +3336,7 @@
       <c r="G38" s="22"/>
       <c r="H38" s="23"/>
       <c r="I38" s="28" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="J38" s="24"/>
       <c r="K38" s="24"/>
@@ -3502,7 +3356,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="19" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B40" s="20" t="n">
         <v>14</v>
@@ -3517,21 +3371,21 @@
       <c r="F40" s="21"/>
       <c r="G40" s="22"/>
       <c r="H40" s="23" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="I40" s="24" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="J40" s="24" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K40" s="24" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="19" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B41" s="20" t="n">
         <v>15</v>
@@ -3546,19 +3400,19 @@
       <c r="F41" s="21"/>
       <c r="G41" s="22"/>
       <c r="H41" s="23" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="I41" s="24" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="J41" s="24" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K41" s="24"/>
     </row>
     <row r="42" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="19" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B42" s="20" t="n">
         <v>16</v>
@@ -3573,19 +3427,19 @@
       <c r="F42" s="21"/>
       <c r="G42" s="22"/>
       <c r="H42" s="23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I42" s="24" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="J42" s="24" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="K42" s="24"/>
     </row>
     <row r="43" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="19" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B43" s="20" t="n">
         <v>17</v>
@@ -3600,19 +3454,19 @@
       <c r="F43" s="21"/>
       <c r="G43" s="22"/>
       <c r="H43" s="23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I43" s="24" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="J43" s="24" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="K43" s="24"/>
     </row>
     <row r="44" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B44" s="20" t="n">
         <v>18</v>
@@ -3627,19 +3481,19 @@
       <c r="F44" s="21"/>
       <c r="G44" s="22"/>
       <c r="H44" s="23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I44" s="24" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="J44" s="24" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="K44" s="24"/>
     </row>
     <row r="45" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="29" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B45" s="20" t="n">
         <v>19</v>
@@ -3654,21 +3508,21 @@
       <c r="F45" s="21"/>
       <c r="G45" s="22"/>
       <c r="H45" s="23" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="I45" s="24" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="J45" s="24" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="K45" s="24" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="29" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B46" s="20" t="n">
         <v>20</v>
@@ -3683,21 +3537,21 @@
       <c r="F46" s="21"/>
       <c r="G46" s="22"/>
       <c r="H46" s="23" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="I46" s="24" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="J46" s="24" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="K46" s="24" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="29" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B47" s="20" t="n">
         <v>21</v>
@@ -3712,21 +3566,21 @@
       <c r="F47" s="21"/>
       <c r="G47" s="22"/>
       <c r="H47" s="23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I47" s="24" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="J47" s="24" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="K47" s="24" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="29" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B48" s="20" t="n">
         <v>22</v>
@@ -3741,16 +3595,16 @@
       <c r="F48" s="21"/>
       <c r="G48" s="22"/>
       <c r="H48" s="23" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I48" s="24" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="J48" s="24" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="K48" s="24" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4480,14 +4334,14 @@
     </row>
     <row r="2" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="32" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B2" s="36" t="n">
         <v>43893</v>
       </c>
       <c r="C2" s="32"/>
       <c r="D2" s="37" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E2" s="32"/>
       <c r="F2" s="34"/>
@@ -4496,7 +4350,7 @@
     </row>
     <row r="3" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="32" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B3" s="36" t="n">
         <f aca="false">B2+21</f>
@@ -4511,10 +4365,10 @@
     </row>
     <row r="4" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="32" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C4" s="32"/>
       <c r="D4" s="32"/>
@@ -4539,7 +4393,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D6" s="32"/>
       <c r="E6" s="32"/>
@@ -4549,7 +4403,7 @@
     </row>
     <row r="7" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="32" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B7" s="32" t="n">
         <f aca="false">COUNTA(D17:D995)</f>
@@ -4564,7 +4418,7 @@
     </row>
     <row r="8" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="32" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B8" s="32" t="n">
         <f aca="false">B7-C8</f>
@@ -4582,7 +4436,7 @@
     </row>
     <row r="9" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="32" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B9" s="32" t="n">
         <f aca="false">B8-C9</f>
@@ -4600,7 +4454,7 @@
     </row>
     <row r="10" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="32" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B10" s="32" t="n">
         <f aca="false">B9-C10</f>
@@ -4618,7 +4472,7 @@
     </row>
     <row r="11" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="32" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B11" s="32" t="n">
         <f aca="false">B10-C11</f>
@@ -4636,7 +4490,7 @@
     </row>
     <row r="12" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="32" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B12" s="32" t="n">
         <f aca="false">B11-C12</f>
@@ -4654,7 +4508,7 @@
     </row>
     <row r="13" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B13" s="32" t="n">
         <f aca="false">B12-C13</f>
@@ -4672,7 +4526,7 @@
     </row>
     <row r="14" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="32" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B14" s="32" t="n">
         <f aca="false">B13-C14</f>
@@ -4700,22 +4554,22 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="40" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B16" s="40" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C16" s="40" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D16" s="40" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="E16" s="40" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F16" s="41" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4723,15 +4577,15 @@
         <v>1</v>
       </c>
       <c r="B17" s="42" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="43" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="E17" s="44"/>
       <c r="F17" s="45" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4739,15 +4593,15 @@
         <v>2</v>
       </c>
       <c r="B18" s="42" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="43" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="E18" s="44"/>
       <c r="F18" s="45" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4755,15 +4609,15 @@
         <v>3</v>
       </c>
       <c r="B19" s="42" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="43" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E19" s="44"/>
       <c r="F19" s="45" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4771,11 +4625,11 @@
         <v>4</v>
       </c>
       <c r="B20" s="42" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="43" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="E20" s="44"/>
       <c r="F20" s="45"/>
@@ -4785,11 +4639,11 @@
         <v>5</v>
       </c>
       <c r="B21" s="42" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="43" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="E21" s="44"/>
       <c r="F21" s="45"/>
@@ -4799,11 +4653,11 @@
         <v>6</v>
       </c>
       <c r="B22" s="42" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="43" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E22" s="44"/>
       <c r="F22" s="45"/>
@@ -4813,11 +4667,11 @@
         <v>7</v>
       </c>
       <c r="B23" s="42" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="43" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E23" s="44"/>
       <c r="F23" s="45"/>
@@ -4827,11 +4681,11 @@
         <v>8</v>
       </c>
       <c r="B24" s="42" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="43" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E24" s="44"/>
       <c r="F24" s="45"/>
@@ -4841,11 +4695,11 @@
         <v>9</v>
       </c>
       <c r="B25" s="42" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="43" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="E25" s="44"/>
       <c r="F25" s="45"/>
@@ -4855,11 +4709,11 @@
         <v>10</v>
       </c>
       <c r="B26" s="42" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="43" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="E26" s="44"/>
       <c r="F26" s="45"/>
@@ -4869,11 +4723,11 @@
         <v>11</v>
       </c>
       <c r="B27" s="42" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="43" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="E27" s="44"/>
       <c r="F27" s="45"/>
@@ -4883,11 +4737,11 @@
         <v>12</v>
       </c>
       <c r="B28" s="42" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="43" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E28" s="44"/>
       <c r="F28" s="45"/>
@@ -4897,11 +4751,11 @@
         <v>13</v>
       </c>
       <c r="B29" s="42" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="43" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="E29" s="44"/>
       <c r="F29" s="45"/>
@@ -4911,11 +4765,11 @@
         <v>14</v>
       </c>
       <c r="B30" s="42" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="43" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="E30" s="44"/>
       <c r="F30" s="45"/>
@@ -4925,11 +4779,11 @@
         <v>15</v>
       </c>
       <c r="B31" s="42" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="43" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="E31" s="44"/>
       <c r="F31" s="45"/>
@@ -4939,11 +4793,11 @@
         <v>16</v>
       </c>
       <c r="B32" s="42" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="43" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E32" s="44"/>
       <c r="F32" s="45"/>
@@ -5642,15 +5496,15 @@
       <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" prompt="Select a Feature ID to the left. Then, in this column, list each discrete task needed to implement that feature.&#10;&#10;Example tasks might be &quot;create the Foo class&quot;, &quot;add the Bar method to the (existing) Qux class&quot;, &quot;Find icons for the task bar&quot;, &quot;Update the manual to cover this feature&quot;, or &quot;Fix the seg fault bug&quot;.&#10;&#10;Expect roughly 3 to 10 tasks per typical feature. Don't OVER plan, but also don't just write &quot;Implement the feature&quot;. Find a middle ground. :-)" promptTitle="Task Description" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D17:D100" type="none">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
     <dataValidation allowBlank="true" error="This cell may only contain a valid status value (hint: use the drop-down selection list) or be left blank (hint: use the Delete key)" errorTitle="Wrong Value" operator="equal" prompt="Leave blank until task is begun.&#10;Select &quot;In Work&quot; when started (for long tasks only).&#10;Select Completed ONLY when this task is done.&#10;    Select &quot;Completed Day 1&quot; if finished on the first day, and&#10;    similarly for &quot;Completed on Day 2&quot; et. al." promptTitle="Implementation Status" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E17:E100" type="list">
       <formula1>"In Work,Completed Day 1,Completed Day 2,Completed Day 3,Completed Day 4,Completed Day 5,Completed Day 6,Completed Day 7"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" prompt="You may add any notes here that help understand the requirements and scope for this task" promptTitle="OPTIONAL" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F17:F100" type="none">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" prompt="Select a Feature ID to the left. Then, in this column, list each discrete task needed to implement that feature.&#10;&#10;Example tasks might be &quot;create the Foo class&quot;, &quot;add the Bar method to the (existing) Qux class&quot;, &quot;Find icons for the task bar&quot;, &quot;Update the manual to cover this feature&quot;, or &quot;Fix the seg fault bug&quot;.&#10;&#10;Expect roughly 3 to 10 tasks per typical feature. Don't OVER plan, but also don't just write &quot;Implement the feature&quot;. Find a middle ground. :-)" promptTitle="Task Description" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D17:D100" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5674,7 +5528,7 @@
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5707,7 +5561,7 @@
     </row>
     <row r="2" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="32" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B2" s="36" t="n">
         <f aca="false">'Sprint 01 Backlog'!B3</f>
@@ -5715,7 +5569,7 @@
       </c>
       <c r="C2" s="32"/>
       <c r="D2" s="37" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E2" s="32"/>
       <c r="F2" s="32"/>
@@ -5724,7 +5578,7 @@
     </row>
     <row r="3" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="32" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B3" s="36" t="n">
         <f aca="false">B2+7</f>
@@ -5739,10 +5593,10 @@
     </row>
     <row r="4" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="32" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C4" s="32"/>
       <c r="D4" s="32"/>
@@ -5767,7 +5621,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D6" s="32"/>
       <c r="E6" s="32"/>
@@ -5777,11 +5631,11 @@
     </row>
     <row r="7" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="32" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B7" s="32" t="n">
         <f aca="false">COUNTA(D17:D995)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C7" s="32"/>
       <c r="D7" s="32"/>
@@ -5792,15 +5646,13 @@
     </row>
     <row r="8" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="32" t="s">
-        <v>115</v>
+        <v>147</v>
       </c>
       <c r="B8" s="32" t="n">
-        <f aca="false">B7-C8</f>
         <v>0</v>
       </c>
       <c r="C8" s="32" t="n">
-        <f aca="false">COUNTIF(E$17:E$995, "Completed Day 1")</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D8" s="32"/>
       <c r="E8" s="32"/>
@@ -5810,15 +5662,13 @@
     </row>
     <row r="9" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="32" t="s">
-        <v>116</v>
+        <v>148</v>
       </c>
       <c r="B9" s="32" t="n">
-        <f aca="false">B8-C9</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C9" s="32" t="n">
-        <f aca="false">COUNTIF(E$17:E$995, "Completed Day 2")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D9" s="32"/>
       <c r="E9" s="32"/>
@@ -5828,11 +5678,11 @@
     </row>
     <row r="10" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="32" t="s">
-        <v>117</v>
+        <v>149</v>
       </c>
       <c r="B10" s="32" t="n">
         <f aca="false">B9-C10</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C10" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -5846,14 +5696,13 @@
     </row>
     <row r="11" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="32" t="s">
-        <v>118</v>
+        <v>150</v>
       </c>
       <c r="B11" s="32" t="n">
-        <f aca="false">B10-C11</f>
-        <v>-2</v>
+        <v>4</v>
       </c>
       <c r="C11" s="32" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D11" s="32"/>
       <c r="E11" s="32"/>
@@ -5863,11 +5712,11 @@
     </row>
     <row r="12" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="32" t="s">
-        <v>119</v>
+        <v>151</v>
       </c>
       <c r="B12" s="32" t="n">
         <f aca="false">B11-C12</f>
-        <v>-2</v>
+        <v>4</v>
       </c>
       <c r="C12" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -5881,11 +5730,11 @@
     </row>
     <row r="13" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
-        <v>120</v>
+        <v>152</v>
       </c>
       <c r="B13" s="32" t="n">
         <f aca="false">B12-C13</f>
-        <v>-2</v>
+        <v>4</v>
       </c>
       <c r="C13" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -5899,15 +5748,13 @@
     </row>
     <row r="14" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="32" t="s">
-        <v>121</v>
+        <v>153</v>
       </c>
       <c r="B14" s="32" t="n">
-        <f aca="false">B13-C14</f>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="C14" s="32" t="n">
-        <f aca="false">COUNTIF(E$17:E$995, "Completed Day 7")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D14" s="32"/>
       <c r="E14" s="32"/>
@@ -5927,69 +5774,77 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="40" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B16" s="40" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C16" s="40" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D16" s="40" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="E16" s="40" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F16" s="40" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B17" s="42" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C17" s="1"/>
-      <c r="D17" s="46"/>
+      <c r="D17" s="46" t="s">
+        <v>154</v>
+      </c>
       <c r="E17" s="44"/>
       <c r="F17" s="45"/>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B18" s="42" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="D18" s="43"/>
+      <c r="D18" s="43" t="s">
+        <v>155</v>
+      </c>
       <c r="E18" s="44"/>
       <c r="F18" s="45"/>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B19" s="42" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="D19" s="43"/>
+      <c r="D19" s="43" t="s">
+        <v>156</v>
+      </c>
       <c r="E19" s="44"/>
       <c r="F19" s="45"/>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B20" s="42" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C20" s="1"/>
-      <c r="D20" s="43"/>
+      <c r="D20" s="43" t="s">
+        <v>157</v>
+      </c>
       <c r="E20" s="44"/>
       <c r="F20" s="45"/>
     </row>
@@ -6872,7 +6727,7 @@
     </row>
     <row r="2" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="32" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B2" s="36" t="n">
         <f aca="false">'Sprint 02 Backlog'!B2+7</f>
@@ -6880,7 +6735,7 @@
       </c>
       <c r="C2" s="32"/>
       <c r="D2" s="37" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E2" s="32"/>
       <c r="F2" s="32"/>
@@ -6889,7 +6744,7 @@
     </row>
     <row r="3" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="32" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B3" s="36" t="n">
         <f aca="false">B2+7</f>
@@ -6904,10 +6759,10 @@
     </row>
     <row r="4" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="32" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C4" s="32"/>
       <c r="D4" s="32"/>
@@ -6932,7 +6787,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D6" s="32"/>
       <c r="E6" s="32"/>
@@ -6942,7 +6797,7 @@
     </row>
     <row r="7" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="32" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B7" s="32" t="n">
         <f aca="false">COUNTA(D17:D995)</f>
@@ -6957,7 +6812,7 @@
     </row>
     <row r="8" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="32" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B8" s="32" t="n">
         <f aca="false">B7-C8</f>
@@ -6975,7 +6830,7 @@
     </row>
     <row r="9" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="32" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B9" s="32" t="n">
         <f aca="false">B8-C9</f>
@@ -6993,7 +6848,7 @@
     </row>
     <row r="10" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="32" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B10" s="32" t="n">
         <f aca="false">B9-C10</f>
@@ -7011,7 +6866,7 @@
     </row>
     <row r="11" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="32" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B11" s="32" t="n">
         <f aca="false">B10-C11</f>
@@ -7029,7 +6884,7 @@
     </row>
     <row r="12" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="32" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B12" s="32" t="n">
         <f aca="false">B11-C12</f>
@@ -7047,7 +6902,7 @@
     </row>
     <row r="13" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B13" s="32" t="n">
         <f aca="false">B12-C13</f>
@@ -7065,7 +6920,7 @@
     </row>
     <row r="14" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="32" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B14" s="32" t="n">
         <f aca="false">B13-C14</f>
@@ -7093,22 +6948,22 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="40" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B16" s="40" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C16" s="40" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D16" s="40" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="E16" s="40" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F16" s="40" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7118,7 +6973,7 @@
       <c r="B17" s="42"/>
       <c r="C17" s="1"/>
       <c r="D17" s="46" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="E17" s="44"/>
       <c r="F17" s="45"/>
@@ -8032,7 +7887,7 @@
     </row>
     <row r="2" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="32" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B2" s="36" t="n">
         <f aca="false">'Sprint 03 Backlog'!B2+14</f>
@@ -8040,7 +7895,7 @@
       </c>
       <c r="C2" s="32"/>
       <c r="D2" s="37" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E2" s="32"/>
       <c r="F2" s="32"/>
@@ -8049,7 +7904,7 @@
     </row>
     <row r="3" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="32" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B3" s="36" t="n">
         <f aca="false">B2+14</f>
@@ -8064,10 +7919,10 @@
     </row>
     <row r="4" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="32" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C4" s="32"/>
       <c r="D4" s="32"/>
@@ -8092,7 +7947,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D6" s="32"/>
       <c r="E6" s="32"/>
@@ -8102,7 +7957,7 @@
     </row>
     <row r="7" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="32" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B7" s="32" t="n">
         <f aca="false">COUNTA(D17:D995)</f>
@@ -8117,7 +7972,7 @@
     </row>
     <row r="8" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="32" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B8" s="32" t="n">
         <f aca="false">B7-C8</f>
@@ -8135,7 +7990,7 @@
     </row>
     <row r="9" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="32" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B9" s="32" t="n">
         <f aca="false">B8-C9</f>
@@ -8153,7 +8008,7 @@
     </row>
     <row r="10" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="32" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B10" s="32" t="n">
         <f aca="false">B9-C10</f>
@@ -8171,7 +8026,7 @@
     </row>
     <row r="11" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="32" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B11" s="32" t="n">
         <f aca="false">B10-C11</f>
@@ -8189,7 +8044,7 @@
     </row>
     <row r="12" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="32" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B12" s="32" t="n">
         <f aca="false">B11-C12</f>
@@ -8207,7 +8062,7 @@
     </row>
     <row r="13" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B13" s="32" t="n">
         <f aca="false">B12-C13</f>
@@ -8225,7 +8080,7 @@
     </row>
     <row r="14" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="32" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B14" s="32" t="n">
         <f aca="false">B13-C14</f>
@@ -8253,22 +8108,22 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="40" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B16" s="40" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C16" s="40" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D16" s="40" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="E16" s="40" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F16" s="40" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8278,11 +8133,11 @@
       <c r="B17" s="42"/>
       <c r="C17" s="1"/>
       <c r="D17" s="46" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="E17" s="44"/>
       <c r="F17" s="45" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>